<commit_message>
Added processor to allow for the conversion of unsynchronized data into synchronized data (DataSet::combine)
</commit_message>
<xml_diff>
--- a/polar-cooordinates-kavi070701.xlsx
+++ b/polar-cooordinates-kavi070701.xlsx
@@ -174,7 +174,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -12793,11 +12793,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="31147717"/>
-        <c:axId val="65028451"/>
+        <c:axId val="22815282"/>
+        <c:axId val="19269371"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="31147717"/>
+        <c:axId val="22815282"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12813,11 +12813,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="65028451"/>
+        <c:crossAx val="19269371"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65028451"/>
+        <c:axId val="19269371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12842,7 +12842,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="31147717"/>
+        <c:crossAx val="22815282"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -12882,15 +12882,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>362520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:colOff>432360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -12898,7 +12898,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1867320" y="36000"/>
+        <a:off x="2223360" y="7560"/>
         <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
@@ -12920,7 +12920,7 @@
   <dimension ref="A1:C1044"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>